<commit_message>
update api aks update view setting ui and profile ui update device status
</commit_message>
<xml_diff>
--- a/Document/Aks.xlsx
+++ b/Document/Aks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mr.Tung\AppNew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\Xamarin\System_aks_vn\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AFCC05-71FA-493A-96C0-2E860358A5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1F0913-708F-4D91-959D-11D15CFBF7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11385" xr2:uid="{0BD4DBFA-E6AC-4E7C-AAA9-627D958E0C8F}"/>
+    <workbookView xWindow="3915" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{0BD4DBFA-E6AC-4E7C-AAA9-627D958E0C8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Chức năng</t>
   </si>
@@ -107,7 +107,22 @@
     <t>#deviceId: D34F4441</t>
   </si>
   <si>
-    <t>token, deviceId</t>
+    <t>#token</t>
+  </si>
+  <si>
+    <t>version, _id, model</t>
+  </si>
+  <si>
+    <t>#token, #deviceId</t>
+  </si>
+  <si>
+    <t>#deviceId</t>
+  </si>
+  <si>
+    <t>"ARM0"</t>
+  </si>
+  <si>
+    <t>remote/getDeviceConfig</t>
   </si>
 </sst>
 </file>
@@ -496,18 +511,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C861D4D9-FC3A-4BC8-ADEB-63711CEC7701}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -565,6 +581,12 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -574,7 +596,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -584,6 +606,9 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -606,8 +631,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>